<commit_message>
Rework bulk change functionality
Splitting the create & update workflow across two sheets, and dealing
with the fact that rows might reference other rows, and that we need
to track dependencies and create everything in the right order.

Rough first version: more cleanup coming soon.
</commit_message>
<xml_diff>
--- a/sample_bulk_edit.xlsx
+++ b/sample_bulk_edit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Records to Create" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
@@ -116,6 +116,33 @@
     <t xml:space="preserve">12/2000</t>
   </si>
   <si>
+    <t xml:space="preserve">approximate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOO123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foo123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copyright_expired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moreton Bay; Aviation; Deafheaven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">something clever</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROW7</t>
   </si>
   <si>
@@ -134,6 +161,9 @@
     <t xml:space="preserve">Paper</t>
   </si>
   <si>
+    <t xml:space="preserve">Z999</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALB</t>
   </si>
   <si>
@@ -149,18 +179,76 @@
     <t xml:space="preserve">USB</t>
   </si>
   <si>
+    <t xml:space="preserve">Compact Disc (CD)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parent</t>
   </si>
   <si>
+    <t xml:space="preserve">ITM100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An AO under an existing one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROW8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physrep under that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physrep under an existing AO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And a digrep too</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Versatile Disc (DVD)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Record QSA ID (ITM, PR, DR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the AO title!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insightful subject; Less insightful subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR11920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the title of a physical representation!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWBOX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the new title for a digital representation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -269,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,6 +379,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,19 +469,19 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.64"/>
@@ -394,7 +490,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="18.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.66"/>
@@ -538,18 +634,53 @@
       <c r="F3" s="0" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>1999</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -558,37 +689,40 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,10 +730,111 @@
         <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="O8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="P8" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>42</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -621,18 +856,18 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.64"/>
@@ -697,7 +932,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -745,12 +980,66 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="J4" s="4"/>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2010</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>43831</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>555</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>666</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="P4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>123</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="P5" s="3"/>
     </row>

</xml_diff>

<commit_message>
Full validation for create & updates
</commit_message>
<xml_diff>
--- a/sample_bulk_edit.xlsx
+++ b/sample_bulk_edit.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t xml:space="preserve">Required</t>
   </si>
@@ -107,150 +107,35 @@
     <t xml:space="preserve">ITM</t>
   </si>
   <si>
-    <t xml:space="preserve">S100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new AO that is pretty good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approximate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOO123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foo123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copyright_expired</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moreton Bay; Aviation; Deafheaven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">something clever</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROW7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Child</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROW3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A PR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROW4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A DR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compact Disc (CD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITM100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An AO under an existing one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROW8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physrep under that</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physrep under an existing AO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">And a digrep too</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Versatile Disc (DVD)</t>
+    <t xml:space="preserve">ITM9999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hooray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLAH333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeah</t>
   </si>
   <si>
     <t xml:space="preserve">Record QSA ID (ITM, PR, DR)</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the AO title!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A new description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insightful subject; Less insightful subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whoa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR11920</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the title of a physical representation!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEWBOX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DR566</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the new title for a digital representation</t>
+    <t xml:space="preserve">PR123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PANTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -285,19 +170,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -357,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,22 +240,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -469,8 +325,8 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,210 +487,25 @@
       <c r="C3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>999</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>1999</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="M4" s="3"/>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>999</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="T8" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -854,16 +525,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.76"/>
@@ -932,7 +603,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -980,69 +651,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>54</v>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2010</v>
-      </c>
-      <c r="G3" s="6" t="n">
-        <v>43831</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>555</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>666</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="P5" s="3"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>